<commit_message>
20220223 Introdução da Roleta
</commit_message>
<xml_diff>
--- a/Dados/Debug/Fitness_Debug.xlsx
+++ b/Dados/Debug/Fitness_Debug.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,542 +464,430 @@
           <t>Resultado Fitness</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>% Acumulada</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cromossoma 39</t>
+          <t>Cromossoma 37</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1230.531685892227</v>
+        <v>1246.69353224093</v>
       </c>
       <c r="D2" t="n">
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F2" t="n">
         <v>83</v>
       </c>
       <c r="G2" t="n">
-        <v>167</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.01995221027479092</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.01995221027479092</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cromossoma 34</t>
+          <t>Cromossoma 31</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1273.107677280289</v>
+        <v>1286.165934192518</v>
       </c>
       <c r="D3" t="n">
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F3" t="n">
         <v>83</v>
       </c>
       <c r="G3" t="n">
-        <v>166</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.01983273596176822</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.03978494623655914</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cromossoma 22</t>
+          <t>Cromossoma 18</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1303.106365549985</v>
+        <v>1306.327057688504</v>
       </c>
       <c r="D4" t="n">
         <v>13</v>
       </c>
       <c r="E4" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F4" t="n">
         <v>84</v>
       </c>
       <c r="G4" t="n">
-        <v>164</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.01959378733572282</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.05937873357228196</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cromossoma 68</t>
+          <t>Cromossoma 48</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1321.106517946048</v>
+        <v>1326.905075558217</v>
       </c>
       <c r="D5" t="n">
         <v>14</v>
       </c>
       <c r="E5" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F5" t="n">
         <v>83</v>
       </c>
       <c r="G5" t="n">
-        <v>160</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.01911589008363202</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.07849462365591398</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cromossoma 25</t>
+          <t>Cromossoma 21</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1345.47547345369</v>
+        <v>1339.011838407931</v>
       </c>
       <c r="D6" t="n">
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F6" t="n">
         <v>83</v>
       </c>
       <c r="G6" t="n">
-        <v>152</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.01816009557945042</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.09665471923536439</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cromossoma 59</t>
+          <t>Cromossoma 71</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1281.143988738227</v>
+        <v>1343.567575776929</v>
       </c>
       <c r="D7" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="n">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F7" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G7" t="n">
-        <v>146</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.01744324970131422</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.1140979689366786</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cromossoma 60</t>
+          <t>Cromossoma 0</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1317.261216227864</v>
+        <v>1356.936496229197</v>
       </c>
       <c r="D8" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="F8" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G8" t="n">
-        <v>143</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.01708482676224612</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.1311827956989247</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cromossoma 72</t>
+          <t>Cromossoma 44</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1318.78718272804</v>
+        <v>1358.562355752864</v>
       </c>
       <c r="D9" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" t="n">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="F9" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G9" t="n">
-        <v>142</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.01696535244922342</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.1481481481481482</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cromossoma 15</t>
+          <t>Cromossoma 72</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1381.814361503866</v>
+        <v>1239.638624029564</v>
       </c>
       <c r="D10" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10" t="n">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="F10" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G10" t="n">
-        <v>140</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.01672640382317802</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.1648745519713262</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cromossoma 47</t>
+          <t>Cromossoma 2</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1327.856005369908</v>
+        <v>1298.811336209352</v>
       </c>
       <c r="D11" t="n">
         <v>15</v>
       </c>
       <c r="E11" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F11" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G11" t="n">
-        <v>140</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.01672640382317802</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.1816009557945042</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cromossoma 52</t>
+          <t>Cromossoma 11</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1382.166860437556</v>
+        <v>1300.8086051789</v>
       </c>
       <c r="D12" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" t="n">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="F12" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G12" t="n">
-        <v>139</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.01660692951015532</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.1982078853046595</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Cromossoma 43</t>
+          <t>Cromossoma 78</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1328.265342744945</v>
+        <v>1305.549187342263</v>
       </c>
       <c r="D13" t="n">
         <v>15</v>
       </c>
       <c r="E13" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F13" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G13" t="n">
-        <v>139</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.01660692951015532</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.2148148148148149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cromossoma 69</t>
+          <t>Cromossoma 19</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1329.142495893582</v>
+        <v>1373.469800497016</v>
       </c>
       <c r="D14" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F14" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G14" t="n">
-        <v>138</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.01648745519713262</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.2313022700119475</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cromossoma 12</t>
+          <t>Cromossoma 23</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1389.789801626789</v>
+        <v>1376.784818087705</v>
       </c>
       <c r="D15" t="n">
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F15" t="n">
         <v>83</v>
       </c>
       <c r="G15" t="n">
-        <v>137</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.01636798088410992</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.2476702508960574</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cromossoma 40</t>
+          <t>Cromossoma 79</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1332.694331231561</v>
+        <v>1309.968537604215</v>
       </c>
       <c r="D16" t="n">
         <v>15</v>
       </c>
       <c r="E16" t="n">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F16" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G16" t="n">
-        <v>137</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.01636798088410992</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0.2640382317801673</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cromossoma 67</t>
+          <t>Cromossoma 63</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1392.906804398118</v>
+        <v>1315.442125115155</v>
       </c>
       <c r="D17" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E17" t="n">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F17" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G17" t="n">
-        <v>136</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.01624850657108722</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.2802867383512546</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cromossoma 45</t>
+          <t>Cromossoma 8</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1334.789330924739</v>
+        <v>1384.419366345562</v>
       </c>
       <c r="D18" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" t="n">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="F18" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G18" t="n">
         <v>136</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.01624850657108722</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.2965352449223418</v>
       </c>
     </row>
     <row r="19">
@@ -1012,1867 +900,1507 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1337.196209088769</v>
+        <v>1388.010367196154</v>
       </c>
       <c r="D19" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" t="n">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="F19" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G19" t="n">
         <v>135</v>
       </c>
-      <c r="H19" t="n">
-        <v>0.01612903225806452</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.3126642771804063</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Cromossoma 31</t>
+          <t>Cromossoma 6</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1339.917467872011</v>
+        <v>1340.829811761365</v>
       </c>
       <c r="D20" t="n">
         <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F20" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G20" t="n">
         <v>134</v>
       </c>
-      <c r="H20" t="n">
-        <v>0.01600955794504182</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0.3286738351254481</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cromossoma 36</t>
+          <t>Cromossoma 39</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1346.622779476705</v>
+        <v>1389.899209511203</v>
       </c>
       <c r="D21" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" t="n">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="F21" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G21" t="n">
-        <v>132</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.01577060931899642</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.3444444444444446</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Cromossoma 65</t>
+          <t>Cromossoma 74</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1397.909076969095</v>
+        <v>1347.84289430556</v>
       </c>
       <c r="D22" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="F22" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G22" t="n">
-        <v>130</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.01553166069295102</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0.3599761051373956</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Cromossoma 71</t>
+          <t>Cromossoma 68</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1398.637877358646</v>
+        <v>1347.924899673408</v>
       </c>
       <c r="D23" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E23" t="n">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="F23" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G23" t="n">
-        <v>129</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.01541218637992832</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0.3753882915173239</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Cromossoma 82</t>
+          <t>Cromossoma 67</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1366.959039200596</v>
+        <v>1402.835787504902</v>
       </c>
       <c r="D24" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" t="n">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F24" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G24" t="n">
-        <v>127</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.01517323775388292</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0.3905615292712068</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cromossoma 23</t>
+          <t>Cromossoma 3</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1370.325727656207</v>
+        <v>1348.088954010506</v>
       </c>
       <c r="D25" t="n">
         <v>15</v>
       </c>
       <c r="E25" t="n">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F25" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G25" t="n">
-        <v>126</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.01505376344086022</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0.405615292712067</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Cromossoma 4</t>
+          <t>Cromossoma 15</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1370.579765028376</v>
+        <v>1349.190783683897</v>
       </c>
       <c r="D26" t="n">
         <v>15</v>
       </c>
       <c r="E26" t="n">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F26" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G26" t="n">
-        <v>125</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.01493428912783751</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0.4205495818399045</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Cromossoma 83</t>
+          <t>Cromossoma 59</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1374.464910200765</v>
+        <v>1351.750729251427</v>
       </c>
       <c r="D27" t="n">
         <v>15</v>
       </c>
       <c r="E27" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F27" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G27" t="n">
-        <v>124</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0.01481481481481482</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0.4353643966547194</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Cromossoma 61</t>
+          <t>Cromossoma 76</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1376.145979340017</v>
+        <v>1352.294532108268</v>
       </c>
       <c r="D28" t="n">
         <v>15</v>
       </c>
       <c r="E28" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F28" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G28" t="n">
-        <v>123</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0.01469534050179211</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0.4500597371565115</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Cromossoma 80</t>
+          <t>Cromossoma 13</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1379.681174057646</v>
+        <v>1416.90505239091</v>
       </c>
       <c r="D29" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" t="n">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F29" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G29" t="n">
-        <v>122</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0.01457586618876941</v>
-      </c>
-      <c r="I29" t="n">
-        <v>0.4646356033452809</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cromossoma 37</t>
+          <t>Cromossoma 53</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1385.777653242232</v>
+        <v>1357.43735294492</v>
       </c>
       <c r="D30" t="n">
         <v>15</v>
       </c>
       <c r="E30" t="n">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F30" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G30" t="n">
-        <v>119</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0.01421744324970131</v>
-      </c>
-      <c r="I30" t="n">
-        <v>0.4788530465949822</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Cromossoma 17</t>
+          <t>Cromossoma 30</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1393.054015898423</v>
+        <v>1359.750634361306</v>
       </c>
       <c r="D31" t="n">
         <v>15</v>
       </c>
       <c r="E31" t="n">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="F31" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G31" t="n">
-        <v>116</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0.01385902031063321</v>
-      </c>
-      <c r="I31" t="n">
-        <v>0.4927120669056154</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Cromossoma 8</t>
+          <t>Cromossoma 34</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1454.963188518592</v>
+        <v>1363.622323928188</v>
       </c>
       <c r="D32" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E32" t="n">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="F32" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G32" t="n">
-        <v>116</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.01385902031063321</v>
-      </c>
-      <c r="I32" t="n">
-        <v>0.5065710872162487</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Cromossoma 41</t>
+          <t>Cromossoma 5</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1459.32945341349</v>
+        <v>1366.059235431582</v>
       </c>
       <c r="D33" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E33" t="n">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="F33" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G33" t="n">
-        <v>114</v>
-      </c>
-      <c r="H33" t="n">
-        <v>0.01362007168458781</v>
-      </c>
-      <c r="I33" t="n">
-        <v>0.5201911589008364</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Cromossoma 51</t>
+          <t>Cromossoma 22</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1396.396244902578</v>
+        <v>1437.964736968611</v>
       </c>
       <c r="D34" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E34" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F34" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G34" t="n">
-        <v>113</v>
-      </c>
-      <c r="H34" t="n">
-        <v>0.01350059737156511</v>
-      </c>
-      <c r="I34" t="n">
-        <v>0.5336917562724015</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Cromossoma 79</t>
+          <t>Cromossoma 1</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1396.86786228308</v>
+        <v>1366.096140096388</v>
       </c>
       <c r="D35" t="n">
         <v>15</v>
       </c>
       <c r="E35" t="n">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F35" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G35" t="n">
-        <v>112</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0.01338112305854241</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0.547072879330944</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Cromossoma 5</t>
+          <t>Cromossoma 62</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1470.988825515411</v>
+        <v>1367.702355892584</v>
       </c>
       <c r="D36" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E36" t="n">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F36" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G36" t="n">
-        <v>110</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0.01314217443249701</v>
-      </c>
-      <c r="I36" t="n">
-        <v>0.5602150537634409</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Cromossoma 75</t>
+          <t>Cromossoma 28</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1420.463294024359</v>
+        <v>1448.215108295616</v>
       </c>
       <c r="D37" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37" t="n">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F37" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G37" t="n">
-        <v>108</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0.01290322580645161</v>
-      </c>
-      <c r="I37" t="n">
-        <v>0.5731182795698926</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Cromossoma 49</t>
+          <t>Cromossoma 64</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1477.122026152162</v>
+        <v>1377.657769502315</v>
       </c>
       <c r="D38" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E38" t="n">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F38" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G38" t="n">
-        <v>108</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0.01290322580645161</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0.5860215053763442</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Cromossoma 44</t>
+          <t>Cromossoma 81</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1423.775287863393</v>
+        <v>1462.383799031938</v>
       </c>
       <c r="D39" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F39" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G39" t="n">
-        <v>107</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0.01278375149342891</v>
-      </c>
-      <c r="I39" t="n">
-        <v>0.5988052568697732</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Cromossoma 56</t>
+          <t>Cromossoma 60</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1481.942194581196</v>
+        <v>1404.832365506239</v>
       </c>
       <c r="D40" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E40" t="n">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F40" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G40" t="n">
-        <v>106</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0.01266427718040621</v>
-      </c>
-      <c r="I40" t="n">
-        <v>0.6114695340501793</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Cromossoma 1</t>
+          <t>Cromossoma 14</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1424.395826207032</v>
+        <v>1408.367137992097</v>
       </c>
       <c r="D41" t="n">
         <v>15</v>
       </c>
       <c r="E41" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F41" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G41" t="n">
         <v>106</v>
       </c>
-      <c r="H41" t="n">
-        <v>0.01266427718040621</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0.6241338112305855</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Cromossoma 30</t>
+          <t>Cromossoma 54</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1482.533236061121</v>
+        <v>1477.503875851735</v>
       </c>
       <c r="D42" t="n">
         <v>14</v>
       </c>
       <c r="E42" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F42" t="n">
         <v>83</v>
       </c>
       <c r="G42" t="n">
-        <v>105</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0.01254480286738351</v>
-      </c>
-      <c r="I42" t="n">
-        <v>0.636678614097969</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Cromossoma 27</t>
+          <t>Cromossoma 33</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1433.296350863239</v>
+        <v>1490.09100124271</v>
       </c>
       <c r="D43" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E43" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="F43" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G43" t="n">
-        <v>104</v>
-      </c>
-      <c r="H43" t="n">
-        <v>0.01242532855436081</v>
-      </c>
-      <c r="I43" t="n">
-        <v>0.6491039426523298</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Cromossoma 48</t>
+          <t>Cromossoma 45</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1437.92839025679</v>
+        <v>1428.852421377391</v>
       </c>
       <c r="D44" t="n">
         <v>15</v>
       </c>
       <c r="E44" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F44" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G44" t="n">
         <v>102</v>
       </c>
-      <c r="H44" t="n">
-        <v>0.01218637992831541</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0.6612903225806452</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Cromossoma 18</t>
+          <t>Cromossoma 25</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1286.053704360415</v>
+        <v>1431.182188980257</v>
       </c>
       <c r="D45" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E45" t="n">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="F45" t="n">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="G45" t="n">
-        <v>102</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0.01218637992831541</v>
-      </c>
-      <c r="I45" t="n">
-        <v>0.6734767025089606</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Cromossoma 19</t>
+          <t>Cromossoma 58</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1452.387181025617</v>
+        <v>1448.607416662378</v>
       </c>
       <c r="D46" t="n">
         <v>15</v>
       </c>
       <c r="E46" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F46" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G46" t="n">
-        <v>100</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0.01194743130227001</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0.6854241338112307</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Cromossoma 24</t>
+          <t>Cromossoma 29</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1498.969236569702</v>
+        <v>1453.879395596126</v>
       </c>
       <c r="D47" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E47" t="n">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="F47" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G47" t="n">
-        <v>100</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0.01194743130227001</v>
-      </c>
-      <c r="I47" t="n">
-        <v>0.6973715651135007</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Cromossoma 35</t>
+          <t>Cromossoma 24</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1499.586629678725</v>
+        <v>1454.236383420116</v>
       </c>
       <c r="D48" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E48" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F48" t="n">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="G48" t="n">
-        <v>99</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0.01182795698924731</v>
-      </c>
-      <c r="I48" t="n">
-        <v>0.7091995221027481</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Cromossoma 55</t>
+          <t>Cromossoma 42</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1452.569906785664</v>
+        <v>1456.551805835634</v>
       </c>
       <c r="D49" t="n">
         <v>15</v>
       </c>
       <c r="E49" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F49" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G49" t="n">
-        <v>99</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0.01182795698924731</v>
-      </c>
-      <c r="I49" t="n">
-        <v>0.7210274790919954</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Cromossoma 77</t>
+          <t>Cromossoma 4</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1501.162106025282</v>
+        <v>1517.632608235457</v>
       </c>
       <c r="D50" t="n">
         <v>14</v>
       </c>
       <c r="E50" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>83</v>
       </c>
       <c r="G50" t="n">
-        <v>98</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0.01170848267622461</v>
-      </c>
-      <c r="I50" t="n">
-        <v>0.73273596176822</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Cromossoma 26</t>
+          <t>Cromossoma 17</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1458.232156362171</v>
+        <v>1456.963716193638</v>
       </c>
       <c r="D51" t="n">
         <v>15</v>
       </c>
       <c r="E51" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F51" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G51" t="n">
-        <v>96</v>
-      </c>
-      <c r="H51" t="n">
-        <v>0.01146953405017921</v>
-      </c>
-      <c r="I51" t="n">
-        <v>0.7442054958183992</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Cromossoma 66</t>
+          <t>Cromossoma 73</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1462.406042671111</v>
+        <v>1521.887952661583</v>
       </c>
       <c r="D52" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E52" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G52" t="n">
-        <v>94</v>
-      </c>
-      <c r="H52" t="n">
-        <v>0.01123058542413381</v>
-      </c>
-      <c r="I52" t="n">
-        <v>0.755436081242533</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Cromossoma 53</t>
+          <t>Cromossoma 49</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1464.84052770061</v>
+        <v>1466.269475876888</v>
       </c>
       <c r="D53" t="n">
         <v>15</v>
       </c>
       <c r="E53" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F53" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G53" t="n">
-        <v>93</v>
-      </c>
-      <c r="H53" t="n">
-        <v>0.01111111111111111</v>
-      </c>
-      <c r="I53" t="n">
-        <v>0.7665471923536441</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Cromossoma 58</t>
+          <t>Cromossoma 38</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1350.259617498034</v>
+        <v>1524.486328030174</v>
       </c>
       <c r="D54" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E54" t="n">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="G54" t="n">
-        <v>88</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0.01051373954599761</v>
-      </c>
-      <c r="I54" t="n">
-        <v>0.7770609318996418</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Cromossoma 28</t>
+          <t>Cromossoma 61</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1479.488031098613</v>
+        <v>1469.856236260534</v>
       </c>
       <c r="D55" t="n">
         <v>15</v>
       </c>
       <c r="E55" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F55" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G55" t="n">
         <v>88</v>
       </c>
-      <c r="H55" t="n">
-        <v>0.01051373954599761</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0.7875746714456394</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Cromossoma 11</t>
+          <t>Cromossoma 7</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1350.933717534751</v>
+        <v>1473.732586591282</v>
       </c>
       <c r="D56" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E56" t="n">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="F56" t="n">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="G56" t="n">
-        <v>87</v>
-      </c>
-      <c r="H56" t="n">
-        <v>0.01039426523297491</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0.7979689366786143</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Cromossoma 29</t>
+          <t>Cromossoma 75</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1361.40038128533</v>
+        <v>1474.576973109887</v>
       </c>
       <c r="D57" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E57" t="n">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="F57" t="n">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="G57" t="n">
         <v>85</v>
       </c>
-      <c r="H57" t="n">
-        <v>0.01015531660692951</v>
-      </c>
-      <c r="I57" t="n">
-        <v>0.8081242532855438</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Cromossoma 74</t>
+          <t>Cromossoma 77</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1497.245082661017</v>
+        <v>1480.371247306452</v>
       </c>
       <c r="D58" t="n">
         <v>15</v>
       </c>
       <c r="E58" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F58" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G58" t="n">
-        <v>82</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0.009796893667861409</v>
-      </c>
-      <c r="I58" t="n">
-        <v>0.8179211469534052</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Cromossoma 57</t>
+          <t>Cromossoma 26</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1501.647076864812</v>
+        <v>1484.35095019833</v>
       </c>
       <c r="D59" t="n">
         <v>15</v>
       </c>
       <c r="E59" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F59" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G59" t="n">
-        <v>78</v>
-      </c>
-      <c r="H59" t="n">
-        <v>0.00931899641577061</v>
-      </c>
-      <c r="I59" t="n">
-        <v>0.8272401433691758</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Cromossoma 7</t>
+          <t>Cromossoma 41</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1505.191059398501</v>
+        <v>1495.390177125059</v>
       </c>
       <c r="D60" t="n">
         <v>15</v>
       </c>
       <c r="E60" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F60" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G60" t="n">
-        <v>77</v>
-      </c>
-      <c r="H60" t="n">
-        <v>0.009199522102747909</v>
-      </c>
-      <c r="I60" t="n">
-        <v>0.8364396654719237</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Cromossoma 16</t>
+          <t>Cromossoma 56</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1506.926024339115</v>
+        <v>1497.084036076073</v>
       </c>
       <c r="D61" t="n">
         <v>15</v>
       </c>
       <c r="E61" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F61" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G61" t="n">
         <v>76</v>
       </c>
-      <c r="H61" t="n">
-        <v>0.00908004778972521</v>
-      </c>
-      <c r="I61" t="n">
-        <v>0.845519713261649</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Cromossoma 50</t>
+          <t>Cromossoma 40</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1513.763394327326</v>
+        <v>1499.563244393373</v>
       </c>
       <c r="D62" t="n">
         <v>15</v>
       </c>
       <c r="E62" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F62" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G62" t="n">
         <v>75</v>
       </c>
-      <c r="H62" t="n">
-        <v>0.008960573476702509</v>
-      </c>
-      <c r="I62" t="n">
-        <v>0.8544802867383515</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Cromossoma 32</t>
+          <t>Cromossoma 10</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1523.521719377319</v>
+        <v>1504.140929033275</v>
       </c>
       <c r="D63" t="n">
         <v>15</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F63" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G63" t="n">
-        <v>73</v>
-      </c>
-      <c r="H63" t="n">
-        <v>0.008721624850657108</v>
-      </c>
-      <c r="I63" t="n">
-        <v>0.8632019115890086</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Cromossoma 78</t>
+          <t>Cromossoma 35</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1393.634074423038</v>
+        <v>1511.161419036824</v>
       </c>
       <c r="D64" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E64" t="n">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="F64" t="n">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="G64" t="n">
         <v>72</v>
       </c>
-      <c r="H64" t="n">
-        <v>0.008602150537634409</v>
-      </c>
-      <c r="I64" t="n">
-        <v>0.871804062126643</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Cromossoma 46</t>
+          <t>Cromossoma 83</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1527.416926061399</v>
+        <v>1377.984266267028</v>
       </c>
       <c r="D65" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F65" t="n">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="G65" t="n">
-        <v>72</v>
-      </c>
-      <c r="H65" t="n">
-        <v>0.008602150537634409</v>
-      </c>
-      <c r="I65" t="n">
-        <v>0.8804062126642773</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Cromossoma 2</t>
+          <t>Cromossoma 55</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1394.529888293561</v>
+        <v>1516.875699941966</v>
       </c>
       <c r="D66" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E66" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="G66" t="n">
         <v>71</v>
       </c>
-      <c r="H66" t="n">
-        <v>0.008482676224611709</v>
-      </c>
-      <c r="I66" t="n">
-        <v>0.8888888888888891</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Cromossoma 33</t>
+          <t>Cromossoma 52</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1530.15809541055</v>
+        <v>1519.939137379757</v>
       </c>
       <c r="D67" t="n">
         <v>15</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G67" t="n">
-        <v>71</v>
-      </c>
-      <c r="H67" t="n">
-        <v>0.008482676224611709</v>
-      </c>
-      <c r="I67" t="n">
-        <v>0.8973715651135008</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Cromossoma 76</t>
+          <t>Cromossoma 27</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1534.141534725658</v>
+        <v>1389.755820045953</v>
       </c>
       <c r="D68" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="F68" t="n">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="G68" t="n">
-        <v>70</v>
-      </c>
-      <c r="H68" t="n">
-        <v>0.008363201911589008</v>
-      </c>
-      <c r="I68" t="n">
-        <v>0.9057347670250898</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Cromossoma 70</t>
+          <t>Cromossoma 47</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1353.528156422031</v>
+        <v>1395.889000040523</v>
       </c>
       <c r="D69" t="n">
+        <v>16</v>
+      </c>
+      <c r="E69" t="n">
+        <v>49</v>
+      </c>
+      <c r="F69" t="n">
         <v>17</v>
       </c>
-      <c r="E69" t="n">
-        <v>65</v>
-      </c>
-      <c r="F69" t="n">
-        <v>3</v>
-      </c>
       <c r="G69" t="n">
-        <v>68</v>
-      </c>
-      <c r="H69" t="n">
-        <v>0.008124253285543608</v>
-      </c>
-      <c r="I69" t="n">
-        <v>0.9138590203106334</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Cromossoma 10</t>
+          <t>Cromossoma 50</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1540.729694979405</v>
+        <v>1534.877874423961</v>
       </c>
       <c r="D70" t="n">
         <v>15</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G70" t="n">
-        <v>67</v>
-      </c>
-      <c r="H70" t="n">
-        <v>0.008004778972520908</v>
-      </c>
-      <c r="I70" t="n">
-        <v>0.9218637992831543</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Cromossoma 73</t>
+          <t>Cromossoma 16</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1409.883601741691</v>
+        <v>1402.983565594889</v>
       </c>
       <c r="D71" t="n">
         <v>16</v>
       </c>
       <c r="E71" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F71" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G71" t="n">
-        <v>66</v>
-      </c>
-      <c r="H71" t="n">
-        <v>0.007885304659498209</v>
-      </c>
-      <c r="I71" t="n">
-        <v>0.9297491039426525</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Cromossoma 38</t>
+          <t>Cromossoma 65</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1622.865682201961</v>
+        <v>1541.754284939055</v>
       </c>
       <c r="D72" t="n">
         <v>15</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
+        <v>61</v>
+      </c>
+      <c r="G72" t="n">
         <v>64</v>
-      </c>
-      <c r="G72" t="n">
-        <v>65</v>
-      </c>
-      <c r="H72" t="n">
-        <v>0.007765830346475508</v>
-      </c>
-      <c r="I72" t="n">
-        <v>0.937514934289128</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Cromossoma 20</t>
+          <t>Cromossoma 46</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1430.587065405743</v>
+        <v>1421.062567168302</v>
       </c>
       <c r="D73" t="n">
         <v>16</v>
       </c>
       <c r="E73" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F73" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G73" t="n">
-        <v>62</v>
-      </c>
-      <c r="H73" t="n">
-        <v>0.007407407407407408</v>
-      </c>
-      <c r="I73" t="n">
-        <v>0.9449223416965354</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Cromossoma 64</t>
+          <t>Cromossoma 66</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1436.124578137121</v>
+        <v>1427.832974518617</v>
       </c>
       <c r="D74" t="n">
         <v>16</v>
       </c>
       <c r="E74" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F74" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G74" t="n">
-        <v>60</v>
-      </c>
-      <c r="H74" t="n">
-        <v>0.007168458781362007</v>
-      </c>
-      <c r="I74" t="n">
-        <v>0.9520908004778974</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Cromossoma 81</t>
+          <t>Cromossoma 69</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1451.804601836752</v>
+        <v>1431.891452320111</v>
       </c>
       <c r="D75" t="n">
         <v>16</v>
       </c>
       <c r="E75" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F75" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G75" t="n">
-        <v>58</v>
-      </c>
-      <c r="H75" t="n">
-        <v>0.006929510155316607</v>
-      </c>
-      <c r="I75" t="n">
-        <v>0.959020310633214</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Cromossoma 42</t>
+          <t>Cromossoma 80</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1453.355518409741</v>
+        <v>1434.187040507855</v>
       </c>
       <c r="D76" t="n">
         <v>16</v>
       </c>
       <c r="E76" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F76" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G76" t="n">
         <v>55</v>
       </c>
-      <c r="H76" t="n">
-        <v>0.006571087216248507</v>
-      </c>
-      <c r="I76" t="n">
-        <v>0.9655913978494626</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Cromossoma 0</t>
+          <t>Cromossoma 12</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1467.869372594515</v>
+        <v>1440.982228084333</v>
       </c>
       <c r="D77" t="n">
         <v>16</v>
       </c>
       <c r="E77" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F77" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G77" t="n">
-        <v>49</v>
-      </c>
-      <c r="H77" t="n">
-        <v>0.005854241338112306</v>
-      </c>
-      <c r="I77" t="n">
-        <v>0.9714456391875749</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Cromossoma 62</t>
+          <t>Cromossoma 70</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>1483.328567024056</v>
+        <v>1472.472009738301</v>
       </c>
       <c r="D78" t="n">
         <v>16</v>
       </c>
       <c r="E78" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F78" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G78" t="n">
-        <v>42</v>
-      </c>
-      <c r="H78" t="n">
-        <v>0.005017921146953405</v>
-      </c>
-      <c r="I78" t="n">
-        <v>0.9764635603345283</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Cromossoma 63</t>
+          <t>Cromossoma 57</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1495.323284676997</v>
+        <v>1488.682912122733</v>
       </c>
       <c r="D79" t="n">
         <v>16</v>
@@ -2881,153 +2409,123 @@
         <v>20</v>
       </c>
       <c r="F79" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G79" t="n">
-        <v>41</v>
-      </c>
-      <c r="H79" t="n">
-        <v>0.004898446833930705</v>
-      </c>
-      <c r="I79" t="n">
-        <v>0.981362007168459</v>
+        <v>37</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Cromossoma 3</t>
+          <t>Cromossoma 20</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1496.380191275057</v>
+        <v>1496.113502027998</v>
       </c>
       <c r="D80" t="n">
         <v>16</v>
       </c>
       <c r="E80" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F80" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G80" t="n">
-        <v>40</v>
-      </c>
-      <c r="H80" t="n">
-        <v>0.004778972520908004</v>
-      </c>
-      <c r="I80" t="n">
-        <v>0.986140979689367</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Cromossoma 21</t>
+          <t>Cromossoma 36</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1471.801088391004</v>
+        <v>1496.693860110721</v>
       </c>
       <c r="D81" t="n">
+        <v>16</v>
+      </c>
+      <c r="E81" t="n">
+        <v>16</v>
+      </c>
+      <c r="F81" t="n">
         <v>17</v>
       </c>
-      <c r="E81" t="n">
-        <v>26</v>
-      </c>
-      <c r="F81" t="n">
-        <v>3</v>
-      </c>
       <c r="G81" t="n">
-        <v>29</v>
-      </c>
-      <c r="H81" t="n">
-        <v>0.003464755077658303</v>
-      </c>
-      <c r="I81" t="n">
-        <v>0.9896057347670253</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Cromossoma 6</t>
+          <t>Cromossoma 51</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1535.631238566393</v>
+        <v>1509.208323942731</v>
       </c>
       <c r="D82" t="n">
         <v>16</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F82" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G82" t="n">
-        <v>26</v>
-      </c>
-      <c r="H82" t="n">
-        <v>0.003106332138590203</v>
-      </c>
-      <c r="I82" t="n">
-        <v>0.9927120669056155</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Cromossoma 13</t>
+          <t>Cromossoma 82</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1537.347888986762</v>
+        <v>1534.045756677422</v>
       </c>
       <c r="D83" t="n">
         <v>16</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G83" t="n">
-        <v>25</v>
-      </c>
-      <c r="H83" t="n">
-        <v>0.002986857825567503</v>
-      </c>
-      <c r="I83" t="n">
-        <v>0.995698924731183</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Cromossoma 54</t>
+          <t>Cromossoma 32</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1581.293098006569</v>
+        <v>1550.550585345446</v>
       </c>
       <c r="D84" t="n">
         <v>16</v>
@@ -3036,47 +2534,35 @@
         <v>2</v>
       </c>
       <c r="F84" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G84" t="n">
-        <v>23</v>
-      </c>
-      <c r="H84" t="n">
-        <v>0.002747909199522103</v>
-      </c>
-      <c r="I84" t="n">
-        <v>0.9984468339307051</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Cromossoma 14</t>
+          <t>Cromossoma 43</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1514.3485480837</v>
+        <v>1560.327357589699</v>
       </c>
       <c r="D85" t="n">
+        <v>16</v>
+      </c>
+      <c r="E85" t="n">
+        <v>1</v>
+      </c>
+      <c r="F85" t="n">
         <v>17</v>
       </c>
-      <c r="E85" t="n">
-        <v>10</v>
-      </c>
-      <c r="F85" t="n">
-        <v>3</v>
-      </c>
       <c r="G85" t="n">
-        <v>13</v>
-      </c>
-      <c r="H85" t="n">
-        <v>0.001553166069295101</v>
-      </c>
-      <c r="I85" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>